<commit_message>
data and helper scripts
</commit_message>
<xml_diff>
--- a/data/referee-performance-jsinuosa.xlsx
+++ b/data/referee-performance-jsinuosa.xlsx
@@ -70,9 +70,6 @@
     <t>File 4</t>
   </si>
   <si>
-    <t>Scaffolds</t>
-  </si>
-  <si>
     <t>Bases</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>ANGSD genotype likelihood file size (compressed)</t>
   </si>
   <si>
-    <t>1.371 GB</t>
-  </si>
-  <si>
     <t>seconds</t>
   </si>
   <si>
@@ -157,7 +151,13 @@
     <t>Size of referee output</t>
   </si>
   <si>
-    <t>time -p angsd -GL 2 -i /N/dc2/scratch/grthomas/qtip/jsinuosa/mapped/SRR5380902-header.bam -ref /N/dc2/scratch/grthomas/qtip/jsinuosa/assembly/Trinity.fasta -minQ 0 -doGlf 4 -out jsinuosa-angsd</t>
+    <t>time -p angsd -GL 2 -i /N/dc2/scratch/grthomas/qtip/jsinuosa/mapped/SRR5380902-sorted.bam -ref /N/dc2/scratch/grthomas/qtip/jsinuosa/assembly/Trinity.fasta -minQ 0 -doGlf 4 -out jsinuosa-angsd</t>
+  </si>
+  <si>
+    <t>912.75 MB</t>
+  </si>
+  <si>
+    <t>Transcripts</t>
   </si>
 </sst>
 </file>
@@ -502,160 +502,161 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6">
-        <v>750.47</v>
+        <v>478.79</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B8">
-        <v>212</v>
+        <v>55567</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>99265117</v>
+        <v>50283993</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10">
-        <v>96250753</v>
+        <v>48791504</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed adding unmapped bug where it only tried the first file
</commit_message>
<xml_diff>
--- a/data/referee-performance-jsinuosa.xlsx
+++ b/data/referee-performance-jsinuosa.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bin\referee\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33540" yWindow="468" windowWidth="28620" windowHeight="16320" activeTab="1"/>
+    <workbookView xWindow="-33540" yWindow="465" windowWidth="28620" windowHeight="16320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="j.sinuosa-info" sheetId="4" r:id="rId1"/>
@@ -281,7 +276,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -316,7 +311,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -531,9 +526,9 @@
       <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -707,29 +702,29 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -1204,6 +1199,18 @@
       <c r="I11" t="s">
         <v>6</v>
       </c>
+      <c r="J11">
+        <v>2.4149417877200002E-3</v>
+      </c>
+      <c r="K11">
+        <v>2.4149417877200002E-3</v>
+      </c>
+      <c r="L11">
+        <v>12.9921875</v>
+      </c>
+      <c r="M11">
+        <v>142.96484375</v>
+      </c>
       <c r="O11">
         <v>4</v>
       </c>
@@ -1236,6 +1243,18 @@
       <c r="I12" t="s">
         <v>7</v>
       </c>
+      <c r="J12">
+        <v>0.48018693924</v>
+      </c>
+      <c r="K12">
+        <v>0.48260188102700002</v>
+      </c>
+      <c r="L12">
+        <v>31.12109375</v>
+      </c>
+      <c r="M12">
+        <v>161.03125</v>
+      </c>
       <c r="O12">
         <v>4</v>
       </c>
@@ -1268,6 +1287,18 @@
       <c r="I13" t="s">
         <v>12</v>
       </c>
+      <c r="J13">
+        <v>0.48099708557100002</v>
+      </c>
+      <c r="K13">
+        <v>0.48341202735900002</v>
+      </c>
+      <c r="L13">
+        <v>31.12109375</v>
+      </c>
+      <c r="M13">
+        <v>161.03125</v>
+      </c>
       <c r="O13">
         <v>4</v>
       </c>
@@ -1300,6 +1331,18 @@
       <c r="I14" t="s">
         <v>13</v>
       </c>
+      <c r="J14">
+        <v>1.68704986572E-3</v>
+      </c>
+      <c r="K14">
+        <v>3016.3362939399999</v>
+      </c>
+      <c r="L14">
+        <v>241.16015625</v>
+      </c>
+      <c r="M14">
+        <v>1103.29296875</v>
+      </c>
       <c r="O14">
         <v>4</v>
       </c>
@@ -1332,6 +1375,18 @@
       <c r="I15" t="s">
         <v>47</v>
       </c>
+      <c r="J15">
+        <v>18.4668970108</v>
+      </c>
+      <c r="K15">
+        <v>3034.80319095</v>
+      </c>
+      <c r="L15">
+        <v>241.17578125</v>
+      </c>
+      <c r="M15">
+        <v>1103.29296875</v>
+      </c>
       <c r="O15">
         <v>4</v>
       </c>
@@ -1364,6 +1419,18 @@
       <c r="I16" t="s">
         <v>48</v>
       </c>
+      <c r="J16">
+        <v>237.360594034</v>
+      </c>
+      <c r="K16">
+        <v>3272.1637849799999</v>
+      </c>
+      <c r="L16">
+        <v>243.4140625</v>
+      </c>
+      <c r="M16">
+        <v>1103.29296875</v>
+      </c>
       <c r="O16">
         <v>4</v>
       </c>
@@ -1395,6 +1462,18 @@
       </c>
       <c r="I17" t="s">
         <v>10</v>
+      </c>
+      <c r="J17">
+        <v>2.8939247131299999E-3</v>
+      </c>
+      <c r="K17">
+        <v>3272.16667891</v>
+      </c>
+      <c r="L17">
+        <v>243.4140625</v>
+      </c>
+      <c r="M17">
+        <v>1103.29296875</v>
       </c>
       <c r="O17">
         <v>4</v>
@@ -1429,14 +1508,14 @@
       <selection activeCell="A2" sqref="A2:B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -2332,14 +2411,14 @@
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
jsin data and run script
</commit_message>
<xml_diff>
--- a/data/referee-performance-jsinuosa.xlsx
+++ b/data/referee-performance-jsinuosa.xlsx
@@ -702,7 +702,7 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,6 +1193,18 @@
       <c r="B11" t="s">
         <v>6</v>
       </c>
+      <c r="C11">
+        <v>8.3379745483399999E-3</v>
+      </c>
+      <c r="D11">
+        <v>8.3379745483399999E-3</v>
+      </c>
+      <c r="E11">
+        <v>12.99609375</v>
+      </c>
+      <c r="F11">
+        <v>143.03515625</v>
+      </c>
       <c r="H11">
         <v>4</v>
       </c>
@@ -1237,6 +1249,18 @@
       <c r="B12" t="s">
         <v>7</v>
       </c>
+      <c r="C12">
+        <v>0.76420497894299999</v>
+      </c>
+      <c r="D12">
+        <v>0.772542953491</v>
+      </c>
+      <c r="E12">
+        <v>31.125</v>
+      </c>
+      <c r="F12">
+        <v>161.03125</v>
+      </c>
       <c r="H12">
         <v>4</v>
       </c>
@@ -1281,6 +1305,18 @@
       <c r="B13" t="s">
         <v>12</v>
       </c>
+      <c r="C13">
+        <v>0.76520609855699995</v>
+      </c>
+      <c r="D13">
+        <v>0.77354407310499995</v>
+      </c>
+      <c r="E13">
+        <v>31.125</v>
+      </c>
+      <c r="F13">
+        <v>161.03125</v>
+      </c>
       <c r="H13">
         <v>4</v>
       </c>
@@ -1325,6 +1361,18 @@
       <c r="B14" t="s">
         <v>13</v>
       </c>
+      <c r="C14">
+        <v>1.34706497192E-3</v>
+      </c>
+      <c r="D14">
+        <v>443.22435212099998</v>
+      </c>
+      <c r="E14">
+        <v>239.01953125</v>
+      </c>
+      <c r="F14">
+        <v>1101.265625</v>
+      </c>
       <c r="H14">
         <v>4</v>
       </c>
@@ -1369,6 +1417,18 @@
       <c r="B15" t="s">
         <v>47</v>
       </c>
+      <c r="C15">
+        <v>36.746198892599999</v>
+      </c>
+      <c r="D15">
+        <v>479.97055101400002</v>
+      </c>
+      <c r="E15">
+        <v>239.03515625</v>
+      </c>
+      <c r="F15">
+        <v>1101.265625</v>
+      </c>
       <c r="H15">
         <v>4</v>
       </c>
@@ -1413,6 +1473,18 @@
       <c r="B16" t="s">
         <v>48</v>
       </c>
+      <c r="C16">
+        <v>254.481251955</v>
+      </c>
+      <c r="D16">
+        <v>734.45180296900003</v>
+      </c>
+      <c r="E16">
+        <v>239.046875</v>
+      </c>
+      <c r="F16">
+        <v>1101.265625</v>
+      </c>
       <c r="H16">
         <v>4</v>
       </c>
@@ -1456,6 +1528,18 @@
       </c>
       <c r="B17" t="s">
         <v>10</v>
+      </c>
+      <c r="C17">
+        <v>3.3550262451199999E-3</v>
+      </c>
+      <c r="D17">
+        <v>734.45515799500004</v>
+      </c>
+      <c r="E17">
+        <v>239.046875</v>
+      </c>
+      <c r="F17">
+        <v>1101.265625</v>
       </c>
       <c r="H17">
         <v>4</v>

</xml_diff>